<commit_message>
j'ai oublie de enregistre le excel
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -15,16 +15,12 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Catégorie</t>
   </si>
@@ -233,6 +229,30 @@
     <t>donc trop lourde
 retarde le chargement de
 la page</t>
+  </si>
+  <si>
+    <t>FAIT</t>
+  </si>
+  <si>
+    <t>mot clé dans image non
+exploité</t>
+  </si>
+  <si>
+    <t>remplacer image par du 
+texte</t>
+  </si>
+  <si>
+    <t>texture inutile page 2</t>
+  </si>
+  <si>
+    <t>ralentit chargement de la 
+page et mauvais pour le 
+contraste</t>
+  </si>
+  <si>
+    <t>eviter de surcharger en 
+texture pour faire un design non pertinent et penser au
+contraste</t>
   </si>
 </sst>
 </file>
@@ -300,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,9 +329,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -543,7 +560,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -595,7 +612,7 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -604,15 +621,18 @@
       <c r="C2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="8" t="b">
+      <c r="E2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -621,32 +641,35 @@
       <c r="C3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="8" t="b">
+      <c r="E3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="8" t="b">
+      <c r="E4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -655,106 +678,112 @@
       <c r="C5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="8" t="b">
+      <c r="E5" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="8" t="b">
+      <c r="E7" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="8" t="b">
+      <c r="E8" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="8" t="b">
+      <c r="E9" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="8" t="b">
+      <c r="E10" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="8" t="b">
+      <c r="E11" s="7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -772,7 +801,7 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -782,55 +811,58 @@
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E18" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -840,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
@@ -857,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
@@ -867,18 +899,18 @@
       <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -891,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>41</v>
       </c>
@@ -908,34 +940,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ok reste le rapport
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -15,12 +15,11 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>Catégorie</t>
   </si>
@@ -74,9 +73,6 @@
   </si>
   <si>
     <t>mots clés pas exploités</t>
-  </si>
-  <si>
-    <t>img trop grande</t>
   </si>
   <si>
     <t>url page 2</t>
@@ -138,9 +134,6 @@
     <t>pas de mot clé dans l'url</t>
   </si>
   <si>
-    <t>redimensionner img</t>
-  </si>
-  <si>
     <t>"Entreprise" et "Lyon" pas
 assez exploités</t>
   </si>
@@ -231,9 +224,6 @@
 la page</t>
   </si>
   <si>
-    <t>FAIT</t>
-  </si>
-  <si>
     <t>mot clé dans image non
 exploité</t>
   </si>
@@ -253,6 +243,14 @@
     <t>eviter de surcharger en 
 texture pour faire un design non pertinent et penser au
 contraste</t>
+  </si>
+  <si>
+    <t>img trop grande et img
+en format bmp</t>
+  </si>
+  <si>
+    <t>redimensionner img et
+convertir bmp en jpeg</t>
   </si>
 </sst>
 </file>
@@ -560,7 +558,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -619,16 +617,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -639,16 +634,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
@@ -659,13 +651,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -676,13 +668,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -693,16 +685,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -713,13 +702,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -730,13 +719,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -747,16 +736,13 @@
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -767,7 +753,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="7" t="b">
         <v>1</v>
@@ -778,10 +764,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="7" t="b">
         <v>1</v>
@@ -801,207 +787,198 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E20" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="D22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="E23" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="E24" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E25" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E26" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H26" t="s">
+    </row>
+    <row r="27" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E27" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>